<commit_message>
Added Semester Project Code
Semester Project Code
</commit_message>
<xml_diff>
--- a/ReservoirCode2.xlsx
+++ b/ReservoirCode2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharp Student\Documents\WRSA\GAMS\GitHub\CEE-6410-Campana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36F96DBC-58AC-4959-8F14-5153DB868119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7CE8BFB-6CA5-4402-9D77-45F7877D124D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{D204B51E-2937-4597-9A08-0B14A3ED6822}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{08CEACE1-D9F6-492F-ABDB-84FF4EFD1A36}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="18" r:id="rId1"/>
@@ -61,6 +61,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -76,7 +77,7 @@
     <t>(variable)</t>
   </si>
   <si>
-    <t>Flow Per Location Per Time (Volume)</t>
+    <t>Flow Per Location Per Time (Acft per season)</t>
   </si>
   <si>
     <t>Loc</t>
@@ -658,7 +659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7088AA9D-6722-4737-B02F-40EFFFA0551F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA7FBEC-BA0E-4571-9EA7-53A384088D3C}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1041,34 +1042,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" location="bge!A1" display="bge" xr:uid="{832ECCF2-0D3E-40C0-B81A-BAD0934D0E52}"/>
-    <hyperlink ref="A3" location="ble!A1" display="ble" xr:uid="{3F6D3E7B-F7D1-47F2-AB29-B4D53EA5168B}"/>
-    <hyperlink ref="A4" location="c!A1" display="c" xr:uid="{534E8990-1359-43BE-B2D6-2FFB479B634E}"/>
-    <hyperlink ref="A5" location="CLoc!A1" display="CLoc" xr:uid="{90B91846-B3A0-4BEE-B533-E3935943835C}"/>
-    <hyperlink ref="A6" location="FlowIn!A1" display="FlowIn" xr:uid="{5BEAD94C-C902-44B7-859A-B262250F0A1B}"/>
-    <hyperlink ref="A7" location="GFlow_CONSTRAINTS!A1" display="GFlow_CONSTRAINTS" xr:uid="{98163C07-F62D-407A-A41D-BC7C5A6F08DF}"/>
-    <hyperlink ref="A8" location="GLoc!A1" display="GLoc" xr:uid="{2889A2D6-B3E6-4149-9B8E-5DA9D43E7416}"/>
-    <hyperlink ref="A9" location="ILoc!A1" display="ILoc" xr:uid="{342CF955-9BB7-47C0-8D1B-0F6A9AB98025}"/>
-    <hyperlink ref="A10" location="Scalar!A1" display="IResMB" xr:uid="{B41833B3-BE57-41DD-BFA6-76C5F3161BB0}"/>
-    <hyperlink ref="A11" location="Scalar!A1" display="IStore" xr:uid="{20C359FF-07EB-449F-BABC-60E8BD21AC3F}"/>
-    <hyperlink ref="A12" location="LFlow_CONSTRAINTS!A1" display="LFlow_CONSTRAINTS" xr:uid="{53151BB6-DFBE-4F80-AC3A-BB351FC44F80}"/>
-    <hyperlink ref="A13" location="Loc!A1" display="Loc" xr:uid="{E3D70D97-C685-4E08-B041-21DC4F291832}"/>
-    <hyperlink ref="A14" location="PLoc!A1" display="PLoc" xr:uid="{EDF4A27D-6A8E-4866-B801-FBE7229F1C79}"/>
-    <hyperlink ref="A15" location="Scalar!A1" display="PROFIT" xr:uid="{D88B4D3F-A2A3-479D-9694-2A833BD0A7E4}"/>
-    <hyperlink ref="A16" location="ResMB!A1" display="ResMB" xr:uid="{88F0DCFC-D8AB-42FC-BEAD-E8B6179C4768}"/>
-    <hyperlink ref="A17" location="RiverMB!A1" display="RiverMB" xr:uid="{474E31B6-4D96-411F-AA20-3D0B4AB5ABF9}"/>
-    <hyperlink ref="A18" location="Scalar!A1" display="Sustainability" xr:uid="{411DD13D-896C-4441-A6EC-1ED419B47072}"/>
-    <hyperlink ref="A19" location="test!A1" display="test" xr:uid="{5EF88759-54AA-437D-9DCE-A8AC2C2A4526}"/>
-    <hyperlink ref="A20" location="Time!A1" display="Time" xr:uid="{4C23183B-891C-4E73-9ABF-975D16C93CCC}"/>
-    <hyperlink ref="A21" location="Scalar!A1" display="VPROFIT" xr:uid="{F5E2A3EB-2875-4ED3-A443-2DA2E3D1C49A}"/>
-    <hyperlink ref="A22" location="X!A1" display="X" xr:uid="{41C6DDCB-D20A-43F2-B7BE-BBA7C961C738}"/>
+    <hyperlink ref="A2" location="bge!A1" display="bge" xr:uid="{6FB16895-D2F4-479A-8DCF-6061771FB7A9}"/>
+    <hyperlink ref="A3" location="ble!A1" display="ble" xr:uid="{56804C1B-F1A9-46F2-BE21-445C8FDAFC60}"/>
+    <hyperlink ref="A4" location="c!A1" display="c" xr:uid="{B67EEDA0-154E-41AC-B7FB-D52182BD3584}"/>
+    <hyperlink ref="A5" location="CLoc!A1" display="CLoc" xr:uid="{4FA647E1-01B6-451B-A415-ED7FE4828AAB}"/>
+    <hyperlink ref="A6" location="FlowIn!A1" display="FlowIn" xr:uid="{5915F149-2068-4D53-BE64-7D4ECFDC0843}"/>
+    <hyperlink ref="A7" location="GFlow_CONSTRAINTS!A1" display="GFlow_CONSTRAINTS" xr:uid="{C4A6E078-3D5F-4193-B74A-36D6ED707DB5}"/>
+    <hyperlink ref="A8" location="GLoc!A1" display="GLoc" xr:uid="{544E10DE-4373-4467-AF82-20D926D0C676}"/>
+    <hyperlink ref="A9" location="ILoc!A1" display="ILoc" xr:uid="{DA067990-3D11-43DC-AE3E-D12D350CD239}"/>
+    <hyperlink ref="A10" location="Scalar!A1" display="IResMB" xr:uid="{DD0568B4-0F69-4F5E-9D07-4ADF6170757B}"/>
+    <hyperlink ref="A11" location="Scalar!A1" display="IStore" xr:uid="{BFEADCCA-03B3-4534-AFD3-47C55553E65C}"/>
+    <hyperlink ref="A12" location="LFlow_CONSTRAINTS!A1" display="LFlow_CONSTRAINTS" xr:uid="{AF46ADC2-C84C-487F-98B2-19652F5CDF1B}"/>
+    <hyperlink ref="A13" location="Loc!A1" display="Loc" xr:uid="{AB4FB734-B4AF-41CE-AB48-0C7C803C98C4}"/>
+    <hyperlink ref="A14" location="PLoc!A1" display="PLoc" xr:uid="{6FD7510F-79C0-4509-80B7-06AAA3AD4DE1}"/>
+    <hyperlink ref="A15" location="Scalar!A1" display="PROFIT" xr:uid="{49E87E02-7111-4EFA-979C-6330A9593100}"/>
+    <hyperlink ref="A16" location="ResMB!A1" display="ResMB" xr:uid="{4F054147-CC5D-41DD-99D5-6415A4B039CE}"/>
+    <hyperlink ref="A17" location="RiverMB!A1" display="RiverMB" xr:uid="{BF42902E-B629-4D8A-93E2-F75FEA2BC43F}"/>
+    <hyperlink ref="A18" location="Scalar!A1" display="Sustainability" xr:uid="{A3451541-0DB5-4EF5-9AF5-2A9D9872F511}"/>
+    <hyperlink ref="A19" location="test!A1" display="test" xr:uid="{8B38A4A8-F648-4274-BDD1-86D8A16AFAB2}"/>
+    <hyperlink ref="A20" location="Time!A1" display="Time" xr:uid="{67F767C8-3061-4BB7-9CEA-3624A9803F6F}"/>
+    <hyperlink ref="A21" location="Scalar!A1" display="VPROFIT" xr:uid="{CA004128-3432-4B8E-A74A-E62AE746B029}"/>
+    <hyperlink ref="A22" location="X!A1" display="X" xr:uid="{D84353F3-E47C-4B6B-AF5E-6B7D508117A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46853622-94F9-49CB-A81F-ABF6475217E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6F5A5D-8E3A-4F35-92F8-C0F018AEB120}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1105,16 +1106,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A4" xr:uid="{AA4A394A-5266-43C1-94E0-CFCFB58B9790}"/>
+  <autoFilter ref="A3:A4" xr:uid="{43D4920D-E76D-408C-A69D-47754699A73E}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{89E00B29-1019-49F9-A826-089CC358A955}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{A0F338DF-2DD8-4E8F-B132-8C7A25A907A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9ED80C-64AE-402C-867A-C40B3FEFD5B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE9F451-0559-4628-A3E7-C23DB1940543}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1401,16 +1402,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F15" xr:uid="{C867BDED-752D-4CBF-B654-EEA7B499351E}"/>
+  <autoFilter ref="A3:F15" xr:uid="{D78DFD7B-9BAD-435F-AD91-CC6233CAAA8D}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{4D1B8AF8-77B8-4027-AD97-C99EA9658BA6}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{C52C2530-BF9D-43CC-8683-C5C1F1AFC131}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9938881-37D9-4726-890E-ABA915312C05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31EAD56-611C-4983-93F6-26A1FF0A5545}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1467,16 +1468,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A8" xr:uid="{9538ABB5-F71B-4E98-9C8D-9F4FC8372D7E}"/>
+  <autoFilter ref="A3:A8" xr:uid="{1B46F104-A8AF-4371-841A-B9D767834D35}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{E8B66D00-FE86-4CE4-B355-221C31E9130B}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{B350838D-310A-4E0C-9027-DD2E122178BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0B3D96-CF19-4DCA-8ABA-5C6FD22B40BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56990853-AB3D-455D-946A-BCAA5EBA62AA}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1518,16 +1519,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A5" xr:uid="{BBE695B7-7E85-4A71-AD34-D34B95324255}"/>
+  <autoFilter ref="A3:A5" xr:uid="{81BFAA16-F31A-4BD3-8C44-D6B4E145C30C}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{169506A8-54F2-4B01-935A-4F7B4155D236}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{E85E4467-0B93-4253-823C-313FDDFB7E1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECDCC7C-790C-4151-819E-F9A3E021FE97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F635D6-FECD-4389-8132-B29341439516}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1656,16 +1657,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E8" xr:uid="{1B091029-0FA7-40AC-BF51-BD1D08E82006}"/>
+  <autoFilter ref="A3:E8" xr:uid="{1337F229-CDBE-4C67-A2D4-DAE43ECCC9F7}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{7EE0D6C6-978B-4D3A-B29A-6175697D9258}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{24636AD6-2C2C-4FB8-83B5-4CFA76D3E5EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C2917D-F24A-41BE-88C3-4EB546932983}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455EC2EE-F730-4438-B36E-D5518FF1E048}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2312,16 +2313,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F33" xr:uid="{28263E7C-201F-4635-B894-C7053AF93663}"/>
+  <autoFilter ref="A3:F33" xr:uid="{4EB2EEBE-875E-411C-A41F-8B6BAFA22646}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{69B93F7F-4498-430D-A816-41C63577F2F5}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{02DE0CBC-0BAA-4817-BCAF-F297E1B92AEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5428636-9A0E-42B3-9D04-78699A252818}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7954E4F-D25C-4C70-9D57-FABCFE5DEA10}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2396,16 +2397,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B8" xr:uid="{75AFC38F-AC94-42E9-8878-DFFCEF4AC0A8}"/>
+  <autoFilter ref="A3:B8" xr:uid="{8A9A6808-1CEC-4F94-A2FA-CB529A6DEA66}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{365F3F77-03E3-468F-9098-512789A10F1B}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{170A14BC-4D71-4E87-A865-A3A251667561}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE98B36-A068-433E-8CFC-FBD17CA95A35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3335A0-2A13-4740-BD31-5F9724B659A5}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2467,16 +2468,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A9" xr:uid="{C119CB67-0D0D-421B-9DA7-B1F4F1403773}"/>
+  <autoFilter ref="A3:A9" xr:uid="{4AFC63A1-6DC4-4DF6-8567-0F4A0967AEFB}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{0ACD7414-B70A-4FDD-A8D9-BCEB51E0D7E7}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{1EED9284-BF44-45A4-AF56-97C9ABA66BC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA5B700-FF99-4295-A96E-6673B33D8ECE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC8B4DB-8AEC-48BE-9C22-D27CDFD00692}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3123,16 +3124,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F33" xr:uid="{E47A64EB-AAE1-4576-A674-27774C8156CF}"/>
+  <autoFilter ref="A3:F33" xr:uid="{A3B51960-A304-4AE3-9DBC-791BD6F56D73}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{7DE18DB2-9CF6-467C-AC5B-F99577927678}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{8787B2D9-6F6E-46C0-BCB6-E5F485437BE1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A49B820-EC9F-43D8-9EE6-07BE047B82E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9C3EB5-458B-44FD-B836-84988CB24A15}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3288,14 +3289,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{AF8BEA4C-E7CB-4290-8187-183B2FA4B684}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{5D2D3E91-7288-45BE-8B33-9F0A233CDB4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56D5261-3941-4031-99F9-736E17EAA17B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F609AF-141A-40F2-AF92-7D050537C63A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3338,16 +3339,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B4" xr:uid="{470E11D7-FE38-4311-8204-3DD54F94FC42}"/>
+  <autoFilter ref="A3:B4" xr:uid="{EADEC492-431F-4BA2-97DD-2FE77A003C5F}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{E9BBA672-8921-4594-B9C6-3DA0CC3995BD}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{AF4D127A-5DE4-4551-ACD3-D61278B1C3AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C438B5A-4E5E-4EBA-A14A-D362716606A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A2351E-8B02-43D9-8525-D4C77D48D3B4}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3398,16 +3399,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B5" xr:uid="{CECF54CD-7219-4957-A427-CB25FC5C5BCF}"/>
+  <autoFilter ref="A3:B5" xr:uid="{0D8A7A17-9B14-42E4-9065-292BA0D4C691}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{CE0578CF-2754-4662-B2A2-EBDE35F7E3E5}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{B0D9605B-AE5A-44C3-BA0E-F95D24FB60CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA7AC69-799A-4DF9-82C4-166F90AF9BDB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48EB81A-C1D7-4B2D-9A26-2C33F877C288}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3577,16 +3578,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:C15" xr:uid="{222CA81A-0A10-4AB2-ACB2-727C993EBC2D}"/>
+  <autoFilter ref="A3:C15" xr:uid="{72808CB3-F687-414D-BF43-85570D7FF682}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{1FCC4FBD-8D53-4E43-9A9C-E9E985267404}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{17FB8965-CFCF-43F7-9630-5A99F1B9E808}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DA4E3B-BD20-422E-88B4-562D16B9E8AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E2DFE7-DD22-48A0-BD4D-EE5736D14165}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3628,16 +3629,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A5" xr:uid="{6F8E7887-F6DB-4BD0-B142-4F7CF6EEC1FE}"/>
+  <autoFilter ref="A3:A5" xr:uid="{B28EBEA1-DFEA-48FD-AA45-913BB2AF3FB3}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{448884F8-7575-42A0-965A-B21ECC6355D5}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{4EF2340D-A9BE-41E2-9C26-0D6981F67C84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71845C5-4FB8-44D8-A222-5EAE7845A942}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21EB1E70-747D-4628-9E2E-A994A567F537}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3741,16 +3742,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:C9" xr:uid="{4A908C79-C2F2-4E44-97B2-62FCED72D728}"/>
+  <autoFilter ref="A3:C9" xr:uid="{0364D4B3-258C-4FFB-B7D3-1AEC0C192DCC}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{79E5655B-D388-4501-921A-AAAFCADB223F}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{0D8E150E-2454-4162-883E-F43448B7AFE3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA9018D-A4D9-4D34-94B3-878309B9316A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFA6E9E-6B77-45B0-8879-EFEA0951BE68}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3917,16 +3918,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F9" xr:uid="{79C1AE12-A237-4BC6-8F98-AE13292109EF}"/>
+  <autoFilter ref="A3:F9" xr:uid="{CEBFD085-80A4-45FE-8DF3-5524F4481CFE}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{71549CD1-82C8-4816-ADDE-AD81F264DE88}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{75EB1737-419E-461E-91DF-7CAA20AD3C19}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9442918-FE7A-4ADC-A305-F5DA4652AD5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C54FF77-3CB3-4786-80A0-7C7FA4A33344}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3963,9 +3964,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A4" xr:uid="{4C49EB46-9938-4AAA-B358-B11C46EEEB56}"/>
+  <autoFilter ref="A3:A4" xr:uid="{6F0E840C-9536-47F1-9CB7-262840AC2E0A}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{3EF0A92C-41C3-4222-AD73-6B13EB0021A1}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{D5FA85AD-B808-430F-94EF-0CD362790118}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>